<commit_message>
#2 Completing read excel functionality
</commit_message>
<xml_diff>
--- a/excel-reader/src/test/resources/input.xlsx
+++ b/excel-reader/src/test/resources/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delacruz\Projects\java-topics\excel-reader\src\test\java\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delacruz\Projects\java-topics\excel-reader\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,6 +21,26 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -339,34 +359,34 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#2 Changing the return type to array into array
</commit_message>
<xml_diff>
--- a/excel-reader/src/test/resources/input.xlsx
+++ b/excel-reader/src/test/resources/input.xlsx
@@ -24,31 +24,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Ranking</t>
+  </si>
+  <si>
+    <t>josdem</t>
+  </si>
+  <si>
+    <t>joseluis.delacruz@gmail.com</t>
+  </si>
+  <si>
+    <t>eric</t>
+  </si>
+  <si>
+    <t>erich@email.com</t>
+  </si>
+  <si>
+    <t>martin</t>
+  </si>
+  <si>
+    <t>martinv@email.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -71,13 +91,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -356,40 +379,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>